<commit_message>
Created quadrature encoder file and initialized quadrature encoder. getVelocity function not working, not sure if QE was initialized properly.
</commit_message>
<xml_diff>
--- a/pin_planner.xlsx
+++ b/pin_planner.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\bishop_ecpe155_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF5E429-B17A-44D5-A123-8E78F9D9AC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244CEE4A-97D5-42B1-B819-BC9BE3C61DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD028536-933F-454A-A147-B90C7DA5A1E0}"/>
+    <workbookView xWindow="1584" yWindow="732" windowWidth="16428" windowHeight="11508" xr2:uid="{DD028536-933F-454A-A147-B90C7DA5A1E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Tiva Port</t>
   </si>
@@ -95,6 +95,24 @@
   </si>
   <si>
     <t>left, pin3</t>
+  </si>
+  <si>
+    <t>left, pin 2</t>
+  </si>
+  <si>
+    <t>right, pin 2</t>
+  </si>
+  <si>
+    <t>QEI0</t>
+  </si>
+  <si>
+    <t>QEI1</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -449,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CEECFC-B5B0-475B-9DE9-E3875C550B5E}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,6 +592,34 @@
         <v>19</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Pin Planner (following Uri's pins)
</commit_message>
<xml_diff>
--- a/pin_planner.xlsx
+++ b/pin_planner.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\bishop_ecpe155_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244CEE4A-97D5-42B1-B819-BC9BE3C61DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB10C96-D29E-4B75-86B7-FB33537597F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1584" yWindow="732" windowWidth="16428" windowHeight="11508" xr2:uid="{DD028536-933F-454A-A147-B90C7DA5A1E0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD028536-933F-454A-A147-B90C7DA5A1E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Tiva Port</t>
   </si>
@@ -49,70 +49,70 @@
     <t>Functionality</t>
   </si>
   <si>
-    <t>M0PWM0</t>
-  </si>
-  <si>
-    <t>M0PWM1</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
+    <t>right, pin 4</t>
+  </si>
+  <si>
+    <t>left, pin 4</t>
+  </si>
+  <si>
+    <t>Wheel</t>
+  </si>
+  <si>
+    <t>IN2</t>
+  </si>
+  <si>
+    <t>left, pin 5</t>
+  </si>
+  <si>
+    <t>IN1</t>
+  </si>
+  <si>
+    <t>left, pin 6</t>
+  </si>
+  <si>
+    <t>right, pin 5</t>
+  </si>
+  <si>
+    <t>right, pin 6</t>
+  </si>
+  <si>
+    <t>STANDBY</t>
+  </si>
+  <si>
+    <t>left, pin 2</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>QEA</t>
+  </si>
+  <si>
+    <t>QEB</t>
+  </si>
+  <si>
+    <t>left, pin 1</t>
+  </si>
+  <si>
+    <t>pin 3</t>
+  </si>
+  <si>
+    <t>pin3</t>
+  </si>
+  <si>
+    <t>high on both right &amp; left</t>
+  </si>
+  <si>
+    <t>M0PWM2</t>
+  </si>
+  <si>
     <t>D</t>
   </si>
   <si>
-    <t>right, pin 4</t>
-  </si>
-  <si>
-    <t>left, pin 4</t>
-  </si>
-  <si>
-    <t>Wheel</t>
-  </si>
-  <si>
-    <t>IN2</t>
-  </si>
-  <si>
-    <t>left, pin 5</t>
-  </si>
-  <si>
-    <t>IN1</t>
-  </si>
-  <si>
-    <t>left, pin 6</t>
-  </si>
-  <si>
-    <t>right, pin 5</t>
-  </si>
-  <si>
-    <t>right, pin 6</t>
-  </si>
-  <si>
-    <t>STANDBY</t>
-  </si>
-  <si>
-    <t>right, pin 3</t>
-  </si>
-  <si>
-    <t>left, pin3</t>
-  </si>
-  <si>
-    <t>left, pin 2</t>
-  </si>
-  <si>
-    <t>right, pin 2</t>
-  </si>
-  <si>
-    <t>QEI0</t>
-  </si>
-  <si>
-    <t>QEI1</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>F</t>
+    <t>M0PWM7</t>
   </si>
 </sst>
 </file>
@@ -467,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CEECFC-B5B0-475B-9DE9-E3875C550B5E}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,7 +481,7 @@
     <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,135 +492,139 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3">
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6">
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C13" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="D13" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cleaned up some files and updated pin planner. Attempted to add counter to interrupt handler, but failed. Will remove in next commit.
</commit_message>
<xml_diff>
--- a/pin_planner.xlsx
+++ b/pin_planner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\bishop_ecpe155_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCD9683-2A96-4D8E-BD29-06C9A1DEBDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE2EEC9-CF47-4D93-8483-22048587F8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD028536-933F-454A-A147-B90C7DA5A1E0}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>Tiva Port</t>
   </si>
@@ -46,9 +46,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>Functionality</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
     <t>left, pin 4</t>
   </si>
   <si>
-    <t>Wheel</t>
-  </si>
-  <si>
     <t>IN2</t>
   </si>
   <si>
@@ -113,6 +107,39 @@
   </si>
   <si>
     <t>high on both right &amp; left wheels</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Red LED (GPIO Output)</t>
+  </si>
+  <si>
+    <t>Blue LED (GPIO Output)</t>
+  </si>
+  <si>
+    <t>Green LED (GPIO Output)</t>
+  </si>
+  <si>
+    <t>Motor Pin</t>
+  </si>
+  <si>
+    <t>Motor Control</t>
+  </si>
+  <si>
+    <t>right, pin 2</t>
+  </si>
+  <si>
+    <t>right, pin 1</t>
+  </si>
+  <si>
+    <t>Set by datasheet</t>
   </si>
 </sst>
 </file>
@@ -467,18 +494,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CEECFC-B5B0-475B-9DE9-E3875C550B5E}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -489,141 +518,196 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="1">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="E18" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B11">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B12">
+      <c r="E19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
         <v>3</v>
       </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
+      <c r="E20" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned up comments and moved count initialization to initQEInterrupt
</commit_message>
<xml_diff>
--- a/pin_planner.xlsx
+++ b/pin_planner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\bishop_ecpe155_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE2EEC9-CF47-4D93-8483-22048587F8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEADCC15-FF23-4E10-89F7-DE9BB9C6FBE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD028536-933F-454A-A147-B90C7DA5A1E0}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Tiva Port</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Set by datasheet</t>
+  </si>
+  <si>
+    <t>previously on PA4, but disconnected bc no need</t>
   </si>
 </sst>
 </file>
@@ -497,7 +500,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -657,17 +660,20 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="1">
-        <v>4</v>
-      </c>
       <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="F14" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
created LED files to initialize LEDs and display LEDs using fucntions. Created bumper sensor files. Currently only accounts for left bumper. created Lab 4 and updated interrupt.c
</commit_message>
<xml_diff>
--- a/pin_planner.xlsx
+++ b/pin_planner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\bishop_ecpe155_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEADCC15-FF23-4E10-89F7-DE9BB9C6FBE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66D67F0-E6E2-4DC5-B0D8-626FAC944F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD028536-933F-454A-A147-B90C7DA5A1E0}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Tiva Port</t>
   </si>
@@ -143,14 +143,31 @@
   </si>
   <si>
     <t>previously on PA4, but disconnected bc no need</t>
+  </si>
+  <si>
+    <t>Bump Sensor</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -178,11 +195,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CEECFC-B5B0-475B-9DE9-E3875C550B5E}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,30 +531,34 @@
     <col min="3" max="3" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="44.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -546,11 +571,11 @@
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -563,11 +588,11 @@
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -581,7 +606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -592,7 +617,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -603,7 +628,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>5</v>
       </c>
@@ -614,7 +639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -627,11 +652,11 @@
       <c r="D10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>7</v>
       </c>
@@ -641,11 +666,11 @@
       <c r="D11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -659,18 +684,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>2</v>
       </c>
@@ -681,7 +706,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C16" s="1" t="s">
         <v>16</v>
       </c>
@@ -689,7 +714,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -700,7 +725,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>2</v>
       </c>
@@ -708,12 +733,31 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>3</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1">
+        <v>6</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="1">
+        <v>7</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
switched bumper pins to PC6 & PC7. bumpSensor now tests for both pins. If signal recieved by bump sensor, vehicle will stop briefly then continue path as specified in main. Also removed LED initialization in quadEncoder. Next step for bumpsensor: update robot reaction upon recieving signal. In addition to stopping, backup and turn slightly to continue movement.
</commit_message>
<xml_diff>
--- a/pin_planner.xlsx
+++ b/pin_planner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\bishop_ecpe155_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66D67F0-E6E2-4DC5-B0D8-626FAC944F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBC0D34-2455-4AB4-BF7A-297442FB0D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD028536-933F-454A-A147-B90C7DA5A1E0}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Tiva Port</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Bump Sensor</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
   <si>
     <t>Left</t>
@@ -521,7 +524,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,21 +746,21 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="B22" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IR Sensor now returns data. Created Lab5 folder. Updated gitignore. Pin Planner updated with IR sensor pins.
</commit_message>
<xml_diff>
--- a/pin_planner.xlsx
+++ b/pin_planner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\bishop_ecpe155_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBC0D34-2455-4AB4-BF7A-297442FB0D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72971D9A-8252-4EEE-85C5-58F97D26FA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD028536-933F-454A-A147-B90C7DA5A1E0}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>Tiva Port</t>
   </si>
@@ -145,16 +145,16 @@
     <t>previously on PA4, but disconnected bc no need</t>
   </si>
   <si>
-    <t>Bump Sensor</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
-    <t>Left</t>
-  </si>
-  <si>
-    <t>Right</t>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>3.3 V</t>
+  </si>
+  <si>
+    <t>5V</t>
   </si>
 </sst>
 </file>
@@ -521,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CEECFC-B5B0-475B-9DE9-E3875C550B5E}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,8 +534,8 @@
     <col min="3" max="3" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="44.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" customWidth="1"/>
+    <col min="7" max="7" width="44.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -554,8 +554,8 @@
       <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>36</v>
+      <c r="F1" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>25</v>
@@ -746,12 +746,12 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1">
         <v>7</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" t="s">
         <v>38</v>
       </c>
     </row>
@@ -759,7 +759,34 @@
       <c r="B23" s="1">
         <v>6</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="1">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed PD1 to PD3 bc PD1 is being used for PB7. Sensor1 now works properly. Currently working on updating lab5 main to function as stated in the Lab5 rubric
</commit_message>
<xml_diff>
--- a/pin_planner.xlsx
+++ b/pin_planner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\bishop_ecpe155_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72971D9A-8252-4EEE-85C5-58F97D26FA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E78A46-CFDB-46C6-BA5C-C578228A3C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD028536-933F-454A-A147-B90C7DA5A1E0}"/>
   </bookViews>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CEECFC-B5B0-475B-9DE9-E3875C550B5E}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -776,7 +776,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F26" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Lab5 now includes bumper functionality along with IR sensor abilities. Updated bumpSensor such that both bumpers can be hit at the same time without crashing the system.
</commit_message>
<xml_diff>
--- a/pin_planner.xlsx
+++ b/pin_planner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\bishop_ecpe155_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E78A46-CFDB-46C6-BA5C-C578228A3C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4F5041-B84D-43B5-B9A1-425B56E7A991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD028536-933F-454A-A147-B90C7DA5A1E0}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>Tiva Port</t>
   </si>
@@ -155,6 +155,21 @@
   </si>
   <si>
     <t>5V</t>
+  </si>
+  <si>
+    <t>left bumper</t>
+  </si>
+  <si>
+    <t>right bumper</t>
+  </si>
+  <si>
+    <t>right cam</t>
+  </si>
+  <si>
+    <t>back cam</t>
+  </si>
+  <si>
+    <t>left cam</t>
   </si>
 </sst>
 </file>
@@ -521,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CEECFC-B5B0-475B-9DE9-E3875C550B5E}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -717,7 +732,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -728,7 +743,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>2</v>
       </c>
@@ -736,7 +751,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>3</v>
       </c>
@@ -744,7 +759,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
@@ -754,16 +769,22 @@
       <c r="F22" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
         <v>6</v>
       </c>
       <c r="F23" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
@@ -773,21 +794,30 @@
       <c r="F25" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
         <v>3</v>
       </c>
       <c r="F26" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
         <v>2</v>
       </c>
       <c r="F27" t="s">
         <v>39</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating the pin planner to include front IR sensors
</commit_message>
<xml_diff>
--- a/pin_planner.xlsx
+++ b/pin_planner.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\bishop_ecpe155_2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Materia\2022 Spring\Courses\ECPE-155 Autonomous Robotics\Labs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9350809-40B0-4C27-8C90-7662DD471518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A36BA0-3BAD-451B-A330-50BCDB166C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD028536-933F-454A-A147-B90C7DA5A1E0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DD028536-933F-454A-A147-B90C7DA5A1E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
   <si>
     <t>Tiva Port</t>
   </si>
@@ -163,15 +163,6 @@
     <t>right bumper</t>
   </si>
   <si>
-    <t>right cam</t>
-  </si>
-  <si>
-    <t>back cam</t>
-  </si>
-  <si>
-    <t>left cam</t>
-  </si>
-  <si>
     <t>GPIO14</t>
   </si>
   <si>
@@ -200,6 +191,21 @@
   </si>
   <si>
     <t>U1Tx</t>
+  </si>
+  <si>
+    <t>Front Right IR</t>
+  </si>
+  <si>
+    <t>Front Left IR</t>
+  </si>
+  <si>
+    <t>back IR</t>
+  </si>
+  <si>
+    <t>right IR</t>
+  </si>
+  <si>
+    <t>left IR</t>
   </si>
 </sst>
 </file>
@@ -607,34 +613,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CEECFC-B5B0-475B-9DE9-E3875C550B5E}">
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="44.5546875" style="2" customWidth="1"/>
-    <col min="8" max="10" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="44.5703125" style="2" customWidth="1"/>
+    <col min="8" max="10" width="8.85546875" style="3"/>
     <col min="11" max="11" width="3" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.88671875" style="3"/>
+    <col min="16" max="16" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,29 +663,29 @@
         <v>25</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -708,7 +714,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -737,7 +743,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="K4" s="4">
         <v>5</v>
       </c>
@@ -749,11 +755,11 @@
       </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -776,14 +782,14 @@
         <v>8</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>2</v>
       </c>
@@ -803,14 +809,14 @@
         <v>10</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>4</v>
       </c>
@@ -833,7 +839,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>5</v>
       </c>
@@ -856,7 +862,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="K9" s="4">
         <v>15</v>
       </c>
@@ -870,7 +876,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -899,7 +905,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>7</v>
       </c>
@@ -925,7 +931,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="K12" s="4">
         <v>21</v>
       </c>
@@ -939,7 +945,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -965,7 +971,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
         <v>16</v>
       </c>
@@ -988,7 +994,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>2</v>
       </c>
@@ -1011,7 +1017,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1031,7 +1037,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="K17" s="4">
         <v>31</v>
       </c>
@@ -1045,7 +1051,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -1068,7 +1074,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>2</v>
       </c>
@@ -1088,7 +1094,7 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>3</v>
       </c>
@@ -1108,7 +1114,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="K21" s="4">
         <v>39</v>
       </c>
@@ -1122,7 +1128,7 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>36</v>
       </c>
@@ -1136,7 +1142,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>6</v>
       </c>
@@ -1147,7 +1153,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
@@ -1158,10 +1164,10 @@
         <v>39</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>3</v>
       </c>
@@ -1169,10 +1175,10 @@
         <v>39</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>2</v>
       </c>
@@ -1180,26 +1186,48 @@
         <v>39</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>6</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <v>7</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B31" s="2">
         <v>0</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B30" s="2">
+      <c r="G31" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
         <v>1</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>54</v>
+      <c r="G32" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Local Changes to Function Library
</commit_message>
<xml_diff>
--- a/pin_planner.xlsx
+++ b/pin_planner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Materia\2022 Spring\Courses\ECPE-155 Autonomous Robotics\Labs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A36BA0-3BAD-451B-A330-50BCDB166C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CAD682-8524-4A5E-80D6-232B277D1A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DD028536-933F-454A-A147-B90C7DA5A1E0}"/>
   </bookViews>
@@ -613,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CEECFC-B5B0-475B-9DE9-E3875C550B5E}">
-  <dimension ref="A1:R32"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,155 +863,138 @@
       <c r="R8" s="4"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K9" s="4">
-        <v>15</v>
-      </c>
+      <c r="B9" s="2">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="6">
-        <v>16</v>
-      </c>
+      <c r="O9" s="6"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2">
-        <v>6</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="4">
-        <v>17</v>
-      </c>
+      <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
-      <c r="O10" s="6">
-        <v>18</v>
-      </c>
+      <c r="O10" s="6"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
-        <v>7</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="K11" s="4">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="6">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2">
+        <v>6</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="K12" s="4">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="6">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="B13" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="K13" s="4">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="6">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="K14" s="4">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="6">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="B15" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="K15" s="4">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="6">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
@@ -1022,212 +1005,259 @@
         <v>16</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="K16" s="4">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="6">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="K17" s="4">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="6">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>27</v>
+      <c r="C18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="K18" s="4">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="6">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
-        <v>2</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="K19" s="4">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="6">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="B20" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K20" s="4">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="6">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>2</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K21" s="4">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="6">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="B22" s="2">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K22" s="4">
+        <v>37</v>
+      </c>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="6">
+        <v>38</v>
+      </c>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K23" s="4">
+        <v>39</v>
+      </c>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="6">
+        <v>40</v>
+      </c>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B24" s="2">
         <v>7</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B23" s="2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B25" s="2">
         <v>6</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B27" s="2">
         <v>0</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B26" s="2">
-        <v>3</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B27" s="2">
-        <v>2</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G29" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <v>6</v>
+      </c>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <v>7</v>
+      </c>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="2">
+        <v>5</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="2">
-        <v>0</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B32" s="2">
-        <v>1</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Saving local changes before troubleshooting serial comm
</commit_message>
<xml_diff>
--- a/pin_planner.xlsx
+++ b/pin_planner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Materia\2022 Spring\Courses\ECPE-155 Autonomous Robotics\Labs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CAD682-8524-4A5E-80D6-232B277D1A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75A083D-2990-417E-B1A5-3078DEB65B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DD028536-933F-454A-A147-B90C7DA5A1E0}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
   <si>
     <t>Tiva Port</t>
   </si>
@@ -197,9 +197,6 @@
   </si>
   <si>
     <t>Front Left IR</t>
-  </si>
-  <si>
-    <t>back IR</t>
   </si>
   <si>
     <t>right IR</t>
@@ -229,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,6 +236,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -284,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -299,6 +302,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CEECFC-B5B0-475B-9DE9-E3875C550B5E}">
-  <dimension ref="A1:R35"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,24 +871,28 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
+    <row r="9" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8">
         <v>3</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="K10" s="4"/>
@@ -1182,40 +1195,51 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="8">
         <v>0</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B28" s="2">
+      <c r="G27" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8">
         <v>3</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="2">
+      <c r="G28" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8">
         <v>2</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>54</v>
+      <c r="G29" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -1247,17 +1271,6 @@
       </c>
       <c r="G34" s="2" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="2">
-        <v>5</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushing not working code
</commit_message>
<xml_diff>
--- a/pin_planner.xlsx
+++ b/pin_planner.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Materia\2022 Spring\Courses\ECPE-155 Autonomous Robotics\Labs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\bishop_ecpe155_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CAD682-8524-4A5E-80D6-232B277D1A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6662A9EB-FAFF-4305-89EB-04350EB22D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DD028536-933F-454A-A147-B90C7DA5A1E0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD028536-933F-454A-A147-B90C7DA5A1E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="59">
   <si>
     <t>Tiva Port</t>
   </si>
@@ -187,12 +187,6 @@
     <t>GND</t>
   </si>
   <si>
-    <t>U1Rx</t>
-  </si>
-  <si>
-    <t>U1Tx</t>
-  </si>
-  <si>
     <t>Front Right IR</t>
   </si>
   <si>
@@ -206,6 +200,18 @@
   </si>
   <si>
     <t>left IR</t>
+  </si>
+  <si>
+    <t>U1Tx, yellow</t>
+  </si>
+  <si>
+    <t>U1Rx, green</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Yellow</t>
   </si>
 </sst>
 </file>
@@ -616,31 +622,31 @@
   <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="44.5703125" style="2" customWidth="1"/>
-    <col min="8" max="10" width="8.85546875" style="3"/>
+    <col min="1" max="1" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="44.5546875" style="2" customWidth="1"/>
+    <col min="8" max="10" width="8.88671875" style="3"/>
     <col min="11" max="11" width="3" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.85546875" style="3"/>
+    <col min="16" max="16" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -685,7 +691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -714,7 +720,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -743,7 +749,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="K4" s="4">
         <v>5</v>
       </c>
@@ -759,7 +765,7 @@
       </c>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -787,9 +793,11 @@
       <c r="Q5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="R5" s="4"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R5" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>2</v>
       </c>
@@ -814,9 +822,11 @@
       <c r="Q6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="R6" s="4"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R6" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>4</v>
       </c>
@@ -839,7 +849,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>5</v>
       </c>
@@ -862,7 +872,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>3</v>
       </c>
@@ -870,7 +880,7 @@
         <v>39</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
@@ -881,7 +891,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -891,7 +901,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="K11" s="4">
         <v>15</v>
       </c>
@@ -905,7 +915,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -934,7 +944,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B13" s="2">
         <v>7</v>
       </c>
@@ -960,7 +970,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="K14" s="4">
         <v>21</v>
       </c>
@@ -974,7 +984,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1000,7 +1010,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1023,7 +1033,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <v>2</v>
       </c>
@@ -1046,7 +1056,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1066,7 +1076,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="K19" s="4">
         <v>31</v>
       </c>
@@ -1080,7 +1090,7 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
@@ -1103,7 +1113,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
         <v>2</v>
       </c>
@@ -1123,7 +1133,7 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B22" s="2">
         <v>3</v>
       </c>
@@ -1143,7 +1153,7 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="K23" s="4">
         <v>39</v>
       </c>
@@ -1157,7 +1167,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>36</v>
       </c>
@@ -1171,7 +1181,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B25" s="2">
         <v>6</v>
       </c>
@@ -1182,7 +1192,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -1193,10 +1203,10 @@
         <v>39</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B28" s="2">
         <v>3</v>
       </c>
@@ -1204,10 +1214,10 @@
         <v>39</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B29" s="2">
         <v>2</v>
       </c>
@@ -1215,22 +1225,22 @@
         <v>39</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B30" s="2">
         <v>6</v>
       </c>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B31" s="2">
         <v>7</v>
       </c>
       <c r="G31" s="3"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -1238,18 +1248,18 @@
         <v>0</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B34" s="2">
         <v>1</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B35" s="2">
         <v>5</v>
       </c>
@@ -1257,7 +1267,7 @@
         <v>39</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>